<commit_message>
updated melting temp link, correction biomass checks
</commit_message>
<xml_diff>
--- a/Strain_characterization_1.xlsx
+++ b/Strain_characterization_1.xlsx
@@ -392,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,19 +429,19 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.1076961183609026</v>
+        <v>0.08780734653187353</v>
       </c>
       <c r="E2">
-        <v>0.08416700273737579</v>
+        <v>0.1010832805811541</v>
       </c>
       <c r="F2">
-        <v>0.08339493837825566</v>
+        <v>0.1093337110524943</v>
       </c>
       <c r="G2">
-        <v>0.1080045685138075</v>
+        <v>0.1026821034618838</v>
       </c>
       <c r="H2">
-        <v>0.1004716368600628</v>
+        <v>0.09947664661360828</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -452,19 +452,19 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.1185127237096473</v>
+        <v>0.1650796997948666</v>
       </c>
       <c r="E3">
-        <v>0.07719085101914309</v>
+        <v>0.2078987434905499</v>
       </c>
       <c r="F3">
-        <v>0.2098227294197972</v>
+        <v>0.2226499106490381</v>
       </c>
       <c r="G3">
-        <v>0.1059660478976897</v>
+        <v>0.2016706780724632</v>
       </c>
       <c r="H3">
-        <v>0.1838938372567979</v>
+        <v>0.1851133549113589</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -475,19 +475,19 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>0.1796111505411552</v>
+        <v>0.2147430119016722</v>
       </c>
       <c r="E4">
-        <v>0.09858973680087811</v>
+        <v>0.5804673287180432</v>
       </c>
       <c r="F4">
-        <v>0.3982704540121199</v>
+        <v>0.4838251325658139</v>
       </c>
       <c r="G4">
-        <v>0.1081862463058069</v>
+        <v>0.3585407898414914</v>
       </c>
       <c r="H4">
-        <v>0.4377170700742722</v>
+        <v>0.2632594727896025</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -498,19 +498,19 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>0.1984920509772485</v>
+        <v>0.3240007582858289</v>
       </c>
       <c r="E5">
-        <v>0.08962267645037827</v>
+        <v>0.9969821803959211</v>
       </c>
       <c r="F5">
-        <v>0.8605009777639842</v>
+        <v>1.363317724523315</v>
       </c>
       <c r="G5">
-        <v>0.09856732546060816</v>
+        <v>0.4025729450841162</v>
       </c>
       <c r="H5">
-        <v>0.725218643336657</v>
+        <v>0.6194870177265485</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -521,19 +521,19 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>0.2987049584605557</v>
+        <v>0.3936433470246172</v>
       </c>
       <c r="E6">
-        <v>0.1054935536630802</v>
+        <v>2.660436513663969</v>
       </c>
       <c r="F6">
-        <v>1.705083936300111</v>
+        <v>2.610345271087341</v>
       </c>
       <c r="G6">
-        <v>0.1075635284811231</v>
+        <v>1.386526248164179</v>
       </c>
       <c r="H6">
-        <v>1.784995319560359</v>
+        <v>1.077680826579565</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -544,19 +544,19 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>0.4569236441893548</v>
+        <v>0.7254465769486362</v>
       </c>
       <c r="E7">
-        <v>0.1082047577467268</v>
+        <v>4.645146977012597</v>
       </c>
       <c r="F7">
-        <v>3.441748738874298</v>
+        <v>5.57102525418424</v>
       </c>
       <c r="G7">
-        <v>0.1079032787579698</v>
+        <v>1.91513625692901</v>
       </c>
       <c r="H7">
-        <v>3.104149785186439</v>
+        <v>2.117025613403249</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -567,19 +567,19 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>0.5276339747748383</v>
+        <v>1.003507105245095</v>
       </c>
       <c r="E8">
-        <v>0.09015791903266668</v>
+        <v>13.36387327652776</v>
       </c>
       <c r="F8">
-        <v>7.161993355437054</v>
+        <v>11.59199298387945</v>
       </c>
       <c r="G8">
-        <v>0.09400965256105352</v>
+        <v>4.058500503443154</v>
       </c>
       <c r="H8">
-        <v>5.543611082183865</v>
+        <v>3.207729588331237</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -590,13 +590,19 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>0.7939567409997278</v>
+        <v>1.349112575410881</v>
+      </c>
+      <c r="E9">
+        <v>25.02081840732266</v>
       </c>
       <c r="F9">
-        <v>12.51608560623441</v>
+        <v>23.4110473243999</v>
+      </c>
+      <c r="G9">
+        <v>6.360986690031143</v>
       </c>
       <c r="H9">
-        <v>10.29425069996188</v>
+        <v>6.739947364441908</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -607,13 +613,19 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <v>0.8601272778924844</v>
+        <v>2.186248522546717</v>
+      </c>
+      <c r="E10">
+        <v>43.40046060235991</v>
       </c>
       <c r="F10">
-        <v>18.76617082290558</v>
+        <v>45.7858437659474</v>
+      </c>
+      <c r="G10">
+        <v>12.30219495560454</v>
       </c>
       <c r="H10">
-        <v>17.96929104800104</v>
+        <v>10.44930409113241</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -624,13 +636,19 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>1.20492924003723</v>
+        <v>3.198752599133604</v>
+      </c>
+      <c r="E11">
+        <v>57.13048410848954</v>
       </c>
       <c r="F11">
-        <v>30.28500265680528</v>
+        <v>61.25762810193658</v>
+      </c>
+      <c r="G11">
+        <v>17.96389601398694</v>
       </c>
       <c r="H11">
-        <v>27.22156445246756</v>
+        <v>19.38765871697455</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -641,13 +659,19 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>1.62639075474368</v>
+        <v>4.186947972036784</v>
+      </c>
+      <c r="E12">
+        <v>80.1805123477714</v>
       </c>
       <c r="F12">
-        <v>33.76969271824311</v>
+        <v>73.44644942832721</v>
+      </c>
+      <c r="G12">
+        <v>33.97076600379182</v>
       </c>
       <c r="H12">
-        <v>41.36239868081444</v>
+        <v>27.38395220043523</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -658,13 +682,19 @@
         <v>11</v>
       </c>
       <c r="D13">
-        <v>1.944617315775425</v>
+        <v>6.176861297530487</v>
+      </c>
+      <c r="E13">
+        <v>78.82959964142194</v>
       </c>
       <c r="F13">
-        <v>40.89892808673518</v>
+        <v>72.85849310540705</v>
+      </c>
+      <c r="G13">
+        <v>41.51970587407652</v>
       </c>
       <c r="H13">
-        <v>35.86403889568714</v>
+        <v>46.95908163939916</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -675,13 +705,19 @@
         <v>12</v>
       </c>
       <c r="D14">
-        <v>2.381532533885121</v>
+        <v>9.283331737767252</v>
+      </c>
+      <c r="E14">
+        <v>75.08399306222516</v>
       </c>
       <c r="F14">
-        <v>35.87579843703642</v>
+        <v>90.6056726420493</v>
+      </c>
+      <c r="G14">
+        <v>57.45789938983254</v>
       </c>
       <c r="H14">
-        <v>41.48274903636168</v>
+        <v>58.29611052092868</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -692,13 +728,19 @@
         <v>13</v>
       </c>
       <c r="D15">
-        <v>3.818264147565862</v>
+        <v>13.51369265441063</v>
+      </c>
+      <c r="E15">
+        <v>90.97377000366427</v>
       </c>
       <c r="F15">
-        <v>37.47823835171526</v>
+        <v>84.82732667270469</v>
+      </c>
+      <c r="G15">
+        <v>74.21397003529698</v>
       </c>
       <c r="H15">
-        <v>42.99070805568468</v>
+        <v>76.65823657345581</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -709,13 +751,19 @@
         <v>14</v>
       </c>
       <c r="D16">
-        <v>4.391201565676617</v>
+        <v>15.7721582079094</v>
+      </c>
+      <c r="E16">
+        <v>104.0632696736731</v>
       </c>
       <c r="F16">
-        <v>40.3877615093439</v>
+        <v>98.02070907111563</v>
+      </c>
+      <c r="G16">
+        <v>80.79742919522283</v>
       </c>
       <c r="H16">
-        <v>42.10044178495438</v>
+        <v>84.79727631776898</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -726,13 +774,19 @@
         <v>15</v>
       </c>
       <c r="D17">
-        <v>4.485635577324262</v>
+        <v>21.70389589637464</v>
+      </c>
+      <c r="E17">
+        <v>102.3854360707015</v>
       </c>
       <c r="F17">
-        <v>48.23644849048112</v>
+        <v>97.89164861323708</v>
+      </c>
+      <c r="G17">
+        <v>89.7481814009232</v>
       </c>
       <c r="H17">
-        <v>46.62050719414642</v>
+        <v>84.22027075055064</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -743,13 +797,19 @@
         <v>16</v>
       </c>
       <c r="D18">
-        <v>6.678738780528265</v>
+        <v>32.68513549368498</v>
+      </c>
+      <c r="E18">
+        <v>95.77875163078022</v>
       </c>
       <c r="F18">
-        <v>42.98150721003876</v>
+        <v>98.25584610521661</v>
+      </c>
+      <c r="G18">
+        <v>84.83760564604884</v>
       </c>
       <c r="H18">
-        <v>47.8051480233453</v>
+        <v>100.4949839530532</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -760,13 +820,19 @@
         <v>17</v>
       </c>
       <c r="D19">
-        <v>9.073643462457097</v>
+        <v>38.81344186938143</v>
+      </c>
+      <c r="E19">
+        <v>92.79265428613898</v>
       </c>
       <c r="F19">
-        <v>45.30807366878021</v>
+        <v>106.0235702795226</v>
+      </c>
+      <c r="G19">
+        <v>84.98864071896837</v>
       </c>
       <c r="H19">
-        <v>45.41510640836411</v>
+        <v>96.69758287210792</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -777,7 +843,13 @@
         <v>18</v>
       </c>
       <c r="D20">
-        <v>10.94744720739829</v>
+        <v>53.45101861405584</v>
+      </c>
+      <c r="G20">
+        <v>87.62503274170679</v>
+      </c>
+      <c r="H20">
+        <v>93.1466030662329</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -788,7 +860,13 @@
         <v>19</v>
       </c>
       <c r="D21">
-        <v>14.23483913044197</v>
+        <v>62.72190269657317</v>
+      </c>
+      <c r="G21">
+        <v>82.10439946224176</v>
+      </c>
+      <c r="H21">
+        <v>85.8365945686314</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -799,7 +877,13 @@
         <v>20</v>
       </c>
       <c r="D22">
-        <v>18.44912001131608</v>
+        <v>62.12743753122583</v>
+      </c>
+      <c r="G22">
+        <v>86.23137960256989</v>
+      </c>
+      <c r="H22">
+        <v>99.34099944987786</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -810,7 +894,13 @@
         <v>21</v>
       </c>
       <c r="D23">
-        <v>18.90220393082588</v>
+        <v>83.32840707379361</v>
+      </c>
+      <c r="G23">
+        <v>112.4449768719314</v>
+      </c>
+      <c r="H23">
+        <v>88.55333137244341</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -821,7 +911,13 @@
         <v>22</v>
       </c>
       <c r="D24">
-        <v>23.68405694325344</v>
+        <v>66.19733555430686</v>
+      </c>
+      <c r="G24">
+        <v>102.5975524646124</v>
+      </c>
+      <c r="H24">
+        <v>101.1631097694899</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -832,7 +928,13 @@
         <v>23</v>
       </c>
       <c r="D25">
-        <v>23.87197827637445</v>
+        <v>90.06294298459825</v>
+      </c>
+      <c r="G25">
+        <v>86.75008776954168</v>
+      </c>
+      <c r="H25">
+        <v>92.29646569528624</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -843,7 +945,7 @@
         <v>24</v>
       </c>
       <c r="D26">
-        <v>28.84002069497343</v>
+        <v>80.14289784026741</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -854,7 +956,7 @@
         <v>25</v>
       </c>
       <c r="D27">
-        <v>34.10251051390046</v>
+        <v>89.29338708514685</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -865,7 +967,7 @@
         <v>26</v>
       </c>
       <c r="D28">
-        <v>33.23212042735565</v>
+        <v>88.82516090437535</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -876,7 +978,7 @@
         <v>27</v>
       </c>
       <c r="D29">
-        <v>41.97076926732446</v>
+        <v>98.82608991189862</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -887,7 +989,7 @@
         <v>28</v>
       </c>
       <c r="D30">
-        <v>34.63452872713577</v>
+        <v>100.0258676077423</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -898,7 +1000,7 @@
         <v>29</v>
       </c>
       <c r="D31">
-        <v>31.78508890797131</v>
+        <v>87.14715091993591</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -909,7 +1011,7 @@
         <v>30</v>
       </c>
       <c r="D32">
-        <v>38.5863348323871</v>
+        <v>89.59159347154952</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -920,7 +1022,7 @@
         <v>31</v>
       </c>
       <c r="D33">
-        <v>46.79358229954043</v>
+        <v>96.49610665229427</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -931,7 +1033,7 @@
         <v>32</v>
       </c>
       <c r="D34">
-        <v>37.30364905666759</v>
+        <v>100.917173918655</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -942,7 +1044,7 @@
         <v>33</v>
       </c>
       <c r="D35">
-        <v>44.79396012545326</v>
+        <v>90.21579073984772</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -953,7 +1055,7 @@
         <v>34</v>
       </c>
       <c r="D36">
-        <v>36.77799517672486</v>
+        <v>96.67339112307776</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -964,7 +1066,7 @@
         <v>35</v>
       </c>
       <c r="D37">
-        <v>40.94915192358532</v>
+        <v>117.0663714263447</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -975,7 +1077,7 @@
         <v>36</v>
       </c>
       <c r="D38">
-        <v>41.12004335013744</v>
+        <v>100.0345409375858</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -986,84 +1088,7 @@
         <v>37</v>
       </c>
       <c r="D39">
-        <v>40.41478644863294</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1">
-        <v>38</v>
-      </c>
-      <c r="B40">
-        <v>38</v>
-      </c>
-      <c r="D40">
-        <v>45.01778910330513</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
-      <c r="B41">
-        <v>39</v>
-      </c>
-      <c r="D41">
-        <v>45.67700105443724</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42">
-        <v>40</v>
-      </c>
-      <c r="D42">
-        <v>44.61078167424156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1">
-        <v>41</v>
-      </c>
-      <c r="B43">
-        <v>41</v>
-      </c>
-      <c r="D43">
-        <v>43.0827256832744</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1">
-        <v>42</v>
-      </c>
-      <c r="B44">
-        <v>42</v>
-      </c>
-      <c r="D44">
-        <v>42.58103008303075</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
-      <c r="B45">
-        <v>43</v>
-      </c>
-      <c r="D45">
-        <v>45.27940973133305</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1">
-        <v>44</v>
-      </c>
-      <c r="B46">
-        <v>44</v>
-      </c>
-      <c r="D46">
-        <v>46.44891065569912</v>
+        <v>86.11419860729993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tm test corrected, figure enabled
</commit_message>
<xml_diff>
--- a/Strain_characterization_1.xlsx
+++ b/Strain_characterization_1.xlsx
@@ -392,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,19 +429,19 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.08780734653187353</v>
+        <v>0.1142586985524135</v>
       </c>
       <c r="E2">
-        <v>0.1010832805811541</v>
+        <v>0.1065029325318719</v>
       </c>
       <c r="F2">
-        <v>0.1093337110524943</v>
+        <v>0.08528972426563008</v>
       </c>
       <c r="G2">
-        <v>0.1026821034618838</v>
+        <v>0.1105213794923197</v>
       </c>
       <c r="H2">
-        <v>0.09947664661360828</v>
+        <v>0.1121894524774864</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -452,19 +452,19 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.1650796997948666</v>
+        <v>0.1187580543085927</v>
       </c>
       <c r="E3">
-        <v>0.2078987434905499</v>
+        <v>0.2141657941562525</v>
       </c>
       <c r="F3">
-        <v>0.2226499106490381</v>
+        <v>0.1673868894695735</v>
       </c>
       <c r="G3">
-        <v>0.2016706780724632</v>
+        <v>0.256203685924516</v>
       </c>
       <c r="H3">
-        <v>0.1851133549113589</v>
+        <v>0.2457789888377989</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -475,19 +475,19 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>0.2147430119016722</v>
+        <v>0.1725693685531227</v>
       </c>
       <c r="E4">
-        <v>0.5804673287180432</v>
+        <v>0.3419621502174148</v>
       </c>
       <c r="F4">
-        <v>0.4838251325658139</v>
+        <v>0.3269998128819627</v>
       </c>
       <c r="G4">
-        <v>0.3585407898414914</v>
+        <v>0.4845143733610661</v>
       </c>
       <c r="H4">
-        <v>0.2632594727896025</v>
+        <v>0.5543580886384267</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -498,19 +498,19 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>0.3240007582858289</v>
+        <v>0.1990363627893637</v>
       </c>
       <c r="E5">
-        <v>0.9969821803959211</v>
+        <v>0.6133483807311121</v>
       </c>
       <c r="F5">
-        <v>1.363317724523315</v>
+        <v>0.7165058510440035</v>
       </c>
       <c r="G5">
-        <v>0.4025729450841162</v>
+        <v>1.377173441754483</v>
       </c>
       <c r="H5">
-        <v>0.6194870177265485</v>
+        <v>1.191427732428485</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -521,19 +521,19 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>0.3936433470246172</v>
+        <v>0.2060247184665036</v>
       </c>
       <c r="E6">
-        <v>2.660436513663969</v>
+        <v>1.06290747902815</v>
       </c>
       <c r="F6">
-        <v>2.610345271087341</v>
+        <v>1.259567647197757</v>
       </c>
       <c r="G6">
-        <v>1.386526248164179</v>
+        <v>1.996983857992604</v>
       </c>
       <c r="H6">
-        <v>1.077680826579565</v>
+        <v>2.865244898738017</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -544,19 +544,19 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>0.7254465769486362</v>
+        <v>0.3020367966961433</v>
       </c>
       <c r="E7">
-        <v>4.645146977012597</v>
+        <v>2.403847289496705</v>
       </c>
       <c r="F7">
-        <v>5.57102525418424</v>
+        <v>1.947104405873099</v>
       </c>
       <c r="G7">
-        <v>1.91513625692901</v>
+        <v>6.336478816774412</v>
       </c>
       <c r="H7">
-        <v>2.117025613403249</v>
+        <v>5.859442856540852</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -567,19 +567,19 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>1.003507105245095</v>
+        <v>0.3440681853332487</v>
       </c>
       <c r="E8">
-        <v>13.36387327652776</v>
+        <v>3.770094562520921</v>
       </c>
       <c r="F8">
-        <v>11.59199298387945</v>
+        <v>3.774921837413167</v>
       </c>
       <c r="G8">
-        <v>4.058500503443154</v>
+        <v>13.88154630555728</v>
       </c>
       <c r="H8">
-        <v>3.207729588331237</v>
+        <v>12.78056414330938</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -590,19 +590,19 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>1.349112575410881</v>
+        <v>0.532300744986195</v>
       </c>
       <c r="E9">
-        <v>25.02081840732266</v>
+        <v>6.143512738541525</v>
       </c>
       <c r="F9">
-        <v>23.4110473243999</v>
+        <v>6.952590901171519</v>
       </c>
       <c r="G9">
-        <v>6.360986690031143</v>
+        <v>25.13311559123643</v>
       </c>
       <c r="H9">
-        <v>6.739947364441908</v>
+        <v>25.79522056605397</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -613,19 +613,19 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <v>2.186248522546717</v>
+        <v>0.5385402165298068</v>
       </c>
       <c r="E10">
-        <v>43.40046060235991</v>
+        <v>11.8960194251739</v>
       </c>
       <c r="F10">
-        <v>45.7858437659474</v>
+        <v>10.20541107356204</v>
       </c>
       <c r="G10">
-        <v>12.30219495560454</v>
+        <v>42.27788787617155</v>
       </c>
       <c r="H10">
-        <v>10.44930409113241</v>
+        <v>39.88653473205823</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -636,19 +636,19 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>3.198752599133604</v>
+        <v>0.6510933183425628</v>
       </c>
       <c r="E11">
-        <v>57.13048410848954</v>
+        <v>20.26049679386849</v>
       </c>
       <c r="F11">
-        <v>61.25762810193658</v>
+        <v>22.65766035830179</v>
       </c>
       <c r="G11">
-        <v>17.96389601398694</v>
+        <v>49.99008797771357</v>
       </c>
       <c r="H11">
-        <v>19.38765871697455</v>
+        <v>54.54728033762993</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -659,19 +659,19 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>4.186947972036784</v>
+        <v>0.665021419322003</v>
       </c>
       <c r="E12">
-        <v>80.1805123477714</v>
+        <v>30.03083656705767</v>
       </c>
       <c r="F12">
-        <v>73.44644942832721</v>
+        <v>27.84439581032989</v>
       </c>
       <c r="G12">
-        <v>33.97076600379182</v>
+        <v>71.48444916046137</v>
       </c>
       <c r="H12">
-        <v>27.38395220043523</v>
+        <v>63.8137482365326</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -682,19 +682,19 @@
         <v>11</v>
       </c>
       <c r="D13">
-        <v>6.176861297530487</v>
+        <v>0.8978264846541173</v>
       </c>
       <c r="E13">
-        <v>78.82959964142194</v>
+        <v>44.27852814319333</v>
       </c>
       <c r="F13">
-        <v>72.85849310540705</v>
+        <v>39.12678193089796</v>
       </c>
       <c r="G13">
-        <v>41.51970587407652</v>
+        <v>74.09910510755705</v>
       </c>
       <c r="H13">
-        <v>46.95908163939916</v>
+        <v>87.26450807714986</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -705,19 +705,19 @@
         <v>12</v>
       </c>
       <c r="D14">
-        <v>9.283331737767252</v>
+        <v>1.033283150342568</v>
       </c>
       <c r="E14">
-        <v>75.08399306222516</v>
+        <v>45.67080936938287</v>
       </c>
       <c r="F14">
-        <v>90.6056726420493</v>
+        <v>59.907607919771</v>
       </c>
       <c r="G14">
-        <v>57.45789938983254</v>
+        <v>90.78618417746785</v>
       </c>
       <c r="H14">
-        <v>58.29611052092868</v>
+        <v>89.54929501879141</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -728,19 +728,19 @@
         <v>13</v>
       </c>
       <c r="D15">
-        <v>13.51369265441063</v>
+        <v>1.263421402216381</v>
       </c>
       <c r="E15">
-        <v>90.97377000366427</v>
+        <v>70.73665541828065</v>
       </c>
       <c r="F15">
-        <v>84.82732667270469</v>
+        <v>60.78965032427504</v>
       </c>
       <c r="G15">
-        <v>74.21397003529698</v>
+        <v>87.98178657913039</v>
       </c>
       <c r="H15">
-        <v>76.65823657345581</v>
+        <v>91.06999213085005</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -751,19 +751,19 @@
         <v>14</v>
       </c>
       <c r="D16">
-        <v>15.7721582079094</v>
+        <v>1.392895266056499</v>
       </c>
       <c r="E16">
-        <v>104.0632696736731</v>
+        <v>73.07330058366908</v>
       </c>
       <c r="F16">
-        <v>98.02070907111563</v>
+        <v>65.84091318132573</v>
       </c>
       <c r="G16">
-        <v>80.79742919522283</v>
+        <v>80.99310163724661</v>
       </c>
       <c r="H16">
-        <v>84.79727631776898</v>
+        <v>96.87109819069866</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -774,19 +774,19 @@
         <v>15</v>
       </c>
       <c r="D17">
-        <v>21.70389589637464</v>
+        <v>1.874790045537552</v>
       </c>
       <c r="E17">
-        <v>102.3854360707015</v>
+        <v>89.65104007731702</v>
       </c>
       <c r="F17">
-        <v>97.89164861323708</v>
+        <v>78.2622059198177</v>
       </c>
       <c r="G17">
-        <v>89.7481814009232</v>
+        <v>78.30611838299704</v>
       </c>
       <c r="H17">
-        <v>84.22027075055064</v>
+        <v>90.61741422682927</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -797,19 +797,19 @@
         <v>16</v>
       </c>
       <c r="D18">
-        <v>32.68513549368498</v>
+        <v>2.582406295991133</v>
       </c>
       <c r="E18">
-        <v>95.77875163078022</v>
+        <v>75.15774815778268</v>
       </c>
       <c r="F18">
-        <v>98.25584610521661</v>
+        <v>81.72342201720647</v>
       </c>
       <c r="G18">
-        <v>84.83760564604884</v>
+        <v>80.98696124132879</v>
       </c>
       <c r="H18">
-        <v>100.4949839530532</v>
+        <v>80.6606642161201</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -820,19 +820,19 @@
         <v>17</v>
       </c>
       <c r="D19">
-        <v>38.81344186938143</v>
+        <v>2.835766969419082</v>
       </c>
       <c r="E19">
-        <v>92.79265428613898</v>
+        <v>85.9569115277357</v>
       </c>
       <c r="F19">
-        <v>106.0235702795226</v>
+        <v>98.33439195760907</v>
       </c>
       <c r="G19">
-        <v>84.98864071896837</v>
+        <v>89.72866519261916</v>
       </c>
       <c r="H19">
-        <v>96.69758287210792</v>
+        <v>85.73051280185452</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -843,13 +843,13 @@
         <v>18</v>
       </c>
       <c r="D20">
-        <v>53.45101861405584</v>
-      </c>
-      <c r="G20">
-        <v>87.62503274170679</v>
-      </c>
-      <c r="H20">
-        <v>93.1466030662329</v>
+        <v>3.273173129454402</v>
+      </c>
+      <c r="E20">
+        <v>87.34119705876086</v>
+      </c>
+      <c r="F20">
+        <v>84.01270653704678</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -860,13 +860,13 @@
         <v>19</v>
       </c>
       <c r="D21">
-        <v>62.72190269657317</v>
-      </c>
-      <c r="G21">
-        <v>82.10439946224176</v>
-      </c>
-      <c r="H21">
-        <v>85.8365945686314</v>
+        <v>3.412741350136176</v>
+      </c>
+      <c r="E21">
+        <v>89.46740484542516</v>
+      </c>
+      <c r="F21">
+        <v>90.03151993377432</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -877,13 +877,13 @@
         <v>20</v>
       </c>
       <c r="D22">
-        <v>62.12743753122583</v>
-      </c>
-      <c r="G22">
-        <v>86.23137960256989</v>
-      </c>
-      <c r="H22">
-        <v>99.34099944987786</v>
+        <v>5.3852799659899</v>
+      </c>
+      <c r="E22">
+        <v>88.17685540040674</v>
+      </c>
+      <c r="F22">
+        <v>80.74747839747401</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -894,13 +894,13 @@
         <v>21</v>
       </c>
       <c r="D23">
-        <v>83.32840707379361</v>
-      </c>
-      <c r="G23">
-        <v>112.4449768719314</v>
-      </c>
-      <c r="H23">
-        <v>88.55333137244341</v>
+        <v>6.042979635111466</v>
+      </c>
+      <c r="E23">
+        <v>96.14246368279656</v>
+      </c>
+      <c r="F23">
+        <v>97.35017504148126</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -911,13 +911,13 @@
         <v>22</v>
       </c>
       <c r="D24">
-        <v>66.19733555430686</v>
-      </c>
-      <c r="G24">
-        <v>102.5975524646124</v>
-      </c>
-      <c r="H24">
-        <v>101.1631097694899</v>
+        <v>5.900160113037796</v>
+      </c>
+      <c r="E24">
+        <v>82.16205014886536</v>
+      </c>
+      <c r="F24">
+        <v>87.04332756701884</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -928,13 +928,13 @@
         <v>23</v>
       </c>
       <c r="D25">
-        <v>90.06294298459825</v>
-      </c>
-      <c r="G25">
-        <v>86.75008776954168</v>
-      </c>
-      <c r="H25">
-        <v>92.29646569528624</v>
+        <v>7.761892011177026</v>
+      </c>
+      <c r="E25">
+        <v>106.7506321427255</v>
+      </c>
+      <c r="F25">
+        <v>79.06541391240165</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -945,7 +945,7 @@
         <v>24</v>
       </c>
       <c r="D26">
-        <v>80.14289784026741</v>
+        <v>10.59995211647931</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -956,7 +956,7 @@
         <v>25</v>
       </c>
       <c r="D27">
-        <v>89.29338708514685</v>
+        <v>12.45388250053755</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -967,7 +967,7 @@
         <v>26</v>
       </c>
       <c r="D28">
-        <v>88.82516090437535</v>
+        <v>13.73740824591042</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -978,7 +978,7 @@
         <v>27</v>
       </c>
       <c r="D29">
-        <v>98.82608991189862</v>
+        <v>13.5592138042465</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -989,7 +989,7 @@
         <v>28</v>
       </c>
       <c r="D30">
-        <v>100.0258676077423</v>
+        <v>18.03862714393862</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1000,7 +1000,7 @@
         <v>29</v>
       </c>
       <c r="D31">
-        <v>87.14715091993591</v>
+        <v>22.90648708505597</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1011,7 +1011,7 @@
         <v>30</v>
       </c>
       <c r="D32">
-        <v>89.59159347154952</v>
+        <v>27.42614979530502</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1022,7 +1022,7 @@
         <v>31</v>
       </c>
       <c r="D33">
-        <v>96.49610665229427</v>
+        <v>26.46724133078785</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1033,7 +1033,7 @@
         <v>32</v>
       </c>
       <c r="D34">
-        <v>100.917173918655</v>
+        <v>34.61380459902725</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1044,7 +1044,7 @@
         <v>33</v>
       </c>
       <c r="D35">
-        <v>90.21579073984772</v>
+        <v>40.25427505071339</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1055,7 +1055,7 @@
         <v>34</v>
       </c>
       <c r="D36">
-        <v>96.67339112307776</v>
+        <v>38.98230435045711</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1066,7 +1066,7 @@
         <v>35</v>
       </c>
       <c r="D37">
-        <v>117.0663714263447</v>
+        <v>43.31366938449019</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1077,7 +1077,7 @@
         <v>36</v>
       </c>
       <c r="D38">
-        <v>100.0345409375858</v>
+        <v>52.98292123012438</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1088,7 +1088,359 @@
         <v>37</v>
       </c>
       <c r="D39">
-        <v>86.11419860729993</v>
+        <v>48.38875170931617</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>38</v>
+      </c>
+      <c r="D40">
+        <v>58.33749036609034</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>39</v>
+      </c>
+      <c r="D41">
+        <v>68.90245716432005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>40</v>
+      </c>
+      <c r="D42">
+        <v>71.97372000110504</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>41</v>
+      </c>
+      <c r="D43">
+        <v>71.5657339775115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>42</v>
+      </c>
+      <c r="D44">
+        <v>64.61622218675642</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>43</v>
+      </c>
+      <c r="D45">
+        <v>66.11605913247193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>44</v>
+      </c>
+      <c r="D46">
+        <v>74.78083973404182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>45</v>
+      </c>
+      <c r="D47">
+        <v>71.26286997381952</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>46</v>
+      </c>
+      <c r="D48">
+        <v>74.63562464915874</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>47</v>
+      </c>
+      <c r="D49">
+        <v>86.62614569471329</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>48</v>
+      </c>
+      <c r="D50">
+        <v>86.06058270085954</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>49</v>
+      </c>
+      <c r="D51">
+        <v>80.24467644362585</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>50</v>
+      </c>
+      <c r="D52">
+        <v>81.92397510831036</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>51</v>
+      </c>
+      <c r="D53">
+        <v>86.34340461651389</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>52</v>
+      </c>
+      <c r="D54">
+        <v>74.55565215089713</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>53</v>
+      </c>
+      <c r="D55">
+        <v>86.73241101452844</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>54</v>
+      </c>
+      <c r="D56">
+        <v>76.69989009450561</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>55</v>
+      </c>
+      <c r="D57">
+        <v>96.84993585147643</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>56</v>
+      </c>
+      <c r="D58">
+        <v>86.80312593206111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>57</v>
+      </c>
+      <c r="D59">
+        <v>90.37439563609601</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>58</v>
+      </c>
+      <c r="D60">
+        <v>85.79923199034162</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>59</v>
+      </c>
+      <c r="D61">
+        <v>82.85300710027032</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>60</v>
+      </c>
+      <c r="D62">
+        <v>89.38287341712579</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>61</v>
+      </c>
+      <c r="D63">
+        <v>91.11236394190499</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>62</v>
+      </c>
+      <c r="D64">
+        <v>99.17707865924018</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>63</v>
+      </c>
+      <c r="D65">
+        <v>95.45427816986368</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>64</v>
+      </c>
+      <c r="D66">
+        <v>83.66023796640106</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>65</v>
+      </c>
+      <c r="D67">
+        <v>89.73924185571688</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>66</v>
+      </c>
+      <c r="D68">
+        <v>100.5520129959937</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>67</v>
+      </c>
+      <c r="D69">
+        <v>93.44211936242009</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>68</v>
+      </c>
+      <c r="D70">
+        <v>83.92095380673342</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>69</v>
+      </c>
+      <c r="D71">
+        <v>74.67877594807399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>